<commit_message>
update images and spreadsheets
</commit_message>
<xml_diff>
--- a/resources/templates/CSF-2.0-profile-template.xlsx
+++ b/resources/templates/CSF-2.0-profile-template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="426" documentId="8_{57FE3F0B-DF34-4D9C-B20E-FF3B2DABBBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79569AB7-A92A-42EE-ADBB-1BDBD4143E9E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{460A6BF6-0421-4064-A645-5D4E89BDBBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{D3338E33-B898-4FA6-A822-4F0A15BCCC45}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="23226" windowHeight="13866" xr2:uid="{D3338E33-B898-4FA6-A822-4F0A15BCCC45}"/>
   </bookViews>
   <sheets>
     <sheet name="Current State" sheetId="6" r:id="rId1"/>
@@ -2936,60 +2936,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">[Any key points to remember including potential challenges or inititives to align with.]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Example: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-- Formalize and publish a mission statement that describes our customers, values, and services.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Elevator pitch characterizing current capabilities across people, process, and technology.]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Example: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-- Employees have a general understanding of the mission and sectors we support.</t>
-    </r>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Cybersecurity Framework 2.0</t>
   </si>
   <si>
     <r>
@@ -3001,7 +2951,7 @@
         <b/>
         <i/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFC00000"/>
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
@@ -3011,7 +2961,7 @@
       <rPr>
         <i/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFC00000"/>
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
@@ -3030,7 +2980,7 @@
         <b/>
         <i/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFC00000"/>
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
@@ -3040,7 +2990,7 @@
       <rPr>
         <i/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFC00000"/>
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
@@ -3049,10 +2999,60 @@
     </r>
   </si>
   <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Cybersecurity Framework 2.0</t>
+    <r>
+      <t xml:space="preserve">[Elevator pitch characterizing current capabilities across people, process, and technology.]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Example: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Employees have a general understanding of the mission and sectors we support.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Any key points to remember including potential challenges or inititives to align with.]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Example: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Formalize and publish a mission statement that describes our customers, values, and services.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3116,17 +3116,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFC00000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFC00000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -3793,10 +3793,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3824,16 +3820,10 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="15" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3852,10 +3842,6 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="21" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3963,6 +3949,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3986,15 +3986,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2576528</xdr:colOff>
+      <xdr:colOff>2557478</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>98939</xdr:rowOff>
+      <xdr:rowOff>135981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>387759</xdr:colOff>
+      <xdr:colOff>366594</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>552064</xdr:rowOff>
+      <xdr:rowOff>512234</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4022,8 +4022,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7326328" y="98939"/>
-          <a:ext cx="607348" cy="455242"/>
+          <a:off x="2557478" y="135981"/>
+          <a:ext cx="473999" cy="374136"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4040,22 +4040,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2576528</xdr:colOff>
+      <xdr:colOff>2561167</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>98939</xdr:rowOff>
+      <xdr:rowOff>143933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>385642</xdr:colOff>
+      <xdr:colOff>373458</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>554181</xdr:rowOff>
+      <xdr:rowOff>519127</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AF0D88B-F408-45ED-819D-2A3E87C1E286}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C781645-EB30-456B-B061-32322BC44F93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4076,8 +4076,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2576528" y="98939"/>
-          <a:ext cx="607348" cy="455242"/>
+          <a:off x="2561167" y="143933"/>
+          <a:ext cx="479291" cy="375194"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4389,96 +4389,96 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" outlineLevelRow="2" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" style="3" customWidth="1"/>
     <col min="2" max="2" width="36" style="3" customWidth="1"/>
     <col min="3" max="3" width="42" style="3" customWidth="1"/>
     <col min="4" max="4" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.703125" style="3"/>
+    <col min="5" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="33"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="88" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="89"/>
-    </row>
-    <row r="3" spans="1:4" s="28" customFormat="1" ht="16.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="87" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="27" t="s">
+      <c r="C2" s="85"/>
+    </row>
+    <row r="3" spans="1:4" s="27" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="83" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="81" t="s">
+    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="102" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="40" t="s">
+    <row r="5" spans="1:4" ht="102" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="134" customHeight="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" ht="134.1" customHeight="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>145</v>
+      <c r="B6" s="88" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>150</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" ref="D6:D67" si="0">LEFT(A6,8)</f>
         <v>GV.OC-01</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OC-02</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>GV.OC-03</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>GV.OC-04</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -4511,18 +4511,18 @@
         <v>GV.OC-05</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="87.5" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="35" t="s">
+    <row r="11" spans="1:4" ht="87.6" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>GV.RM-01</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>GV.RM-02</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>GV.RM-03</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>GV.RM-04</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>GV.RM-05</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>GV.RM-06</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
@@ -4599,18 +4599,18 @@
         <v>GV.RM-07</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="72" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="37" t="s">
+    <row r="19" spans="1:4" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="29"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>GV.RR-01</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>GV.RR-02</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>GV.RR-03</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -4654,18 +4654,18 @@
         <v>GV.RR-04</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="37" t="s">
+    <row r="24" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="29"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>GV.PO-01</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
@@ -4687,18 +4687,18 @@
         <v>GV.PO-02</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="37" t="s">
+    <row r="27" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="30"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>GV.OV-01</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>30</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>GV.OV-02</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>31</v>
       </c>
@@ -4731,18 +4731,18 @@
         <v>GV.OV-03</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="72" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="35" t="s">
+    <row r="31" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="29"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>33</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>GV.SC-01</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>GV.SC-02</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>35</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>GV.SC-03</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>36</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>GV.SC-04</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="72" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" ht="90.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>37</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>GV.SC-05</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>38</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>GV.SC-06</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="72" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" ht="90.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>39</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>GV.SC-07</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>40</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>GV.SC-08</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="72" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" ht="90.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>41</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>GV.SC-09</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>42</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>GV.SC-10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>44</v>
       </c>
@@ -4874,18 +4874,18 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="100.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="35" t="s">
+    <row r="44" spans="1:4" ht="120.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="30"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="29"/>
       <c r="D44" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>ID.AM-01</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>ID.AM-02</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>ID.AM-03</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>ID.AM-04</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>ID.AM-05</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>51</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>ID.AM-07</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>52</v>
       </c>
@@ -4962,18 +4962,18 @@
         <v>ID.AM-08</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="43.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="35" t="s">
+    <row r="52" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="29"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="28"/>
       <c r="D52" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>54</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>ID.RA-01</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>55</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>ID.RA-02</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>56</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>ID.RA-03</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>57</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>ID.RA-04</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>58</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>ID.RA-05</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>59</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>ID.RA-06</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>60</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>ID.RA-07</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>61</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>ID.RA-08</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>62</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>ID.RA-09</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>63</v>
       </c>
@@ -5083,18 +5083,18 @@
         <v>ID.RA-10</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="35" t="s">
+    <row r="63" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="34"/>
-      <c r="C63" s="30"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="29"/>
       <c r="D63" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>65</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>ID.IM-01</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>66</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>ID.IM-02</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>67</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>ID.IM-03</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>68</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>ID.IM-04</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="14.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>69</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>70</v>
       </c>
@@ -5160,18 +5160,18 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="86.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="35" t="s">
+    <row r="70" spans="1:4" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="34"/>
-      <c r="C70" s="30"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="29"/>
       <c r="D70" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>72</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>PR.AA-01</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>73</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>PR.AA-02</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>74</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>PR.AA-03</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>75</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>PR.AA-04</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="72" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>76</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>PR.AA-05</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>77</v>
       </c>
@@ -5237,18 +5237,18 @@
         <v>PR.AA-06</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="72" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="37" t="s">
+    <row r="77" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="36"/>
-      <c r="C77" s="30"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="29"/>
       <c r="D77" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>79</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>PR.AT-01</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>80</v>
       </c>
@@ -5270,18 +5270,18 @@
         <v>PR.AT-02</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="35" t="s">
+    <row r="80" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="36"/>
-      <c r="C80" s="29"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="28"/>
       <c r="D80" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>82</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>PR.DS-01</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>83</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>PR.DS-02</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>84</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>PR.DS-10</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>85</v>
       </c>
@@ -5325,18 +5325,18 @@
         <v>PR.DS-11</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="86.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="35" t="s">
+    <row r="85" spans="1:4" ht="105.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="36"/>
-      <c r="C85" s="29"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="28"/>
       <c r="D85" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>87</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>PR.PS-01</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>88</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>PR.PS-02</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>89</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>PR.PS-03</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
         <v>90</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>PR.PS-04</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>91</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>PR.PS-05</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>92</v>
       </c>
@@ -5402,18 +5402,18 @@
         <v>PR.PS-06</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="72" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="35" t="s">
+    <row r="92" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="34"/>
-      <c r="C92" s="30"/>
+      <c r="B92" s="33"/>
+      <c r="C92" s="29"/>
       <c r="D92" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
         <v>94</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>PR.IR-01</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7" t="s">
         <v>95</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>PR.IR-02</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>96</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>PR.IR-03</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>97</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>PR.IR-04</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="14.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="11" t="s">
         <v>98</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
         <v>99</v>
       </c>
@@ -5479,18 +5479,18 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="35" t="s">
+    <row r="99" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="36"/>
-      <c r="C99" s="29"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="28"/>
       <c r="D99" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
         <v>101</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>DE.CM-01</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
         <v>102</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>DE.CM-02</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
         <v>103</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>DE.CM-03</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
         <v>104</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>DE.CM-06</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
         <v>105</v>
       </c>
@@ -5545,18 +5545,18 @@
         <v>DE.CM-09</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="35" t="s">
+    <row r="105" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="B105" s="34"/>
-      <c r="C105" s="30"/>
+      <c r="B105" s="33"/>
+      <c r="C105" s="29"/>
       <c r="D105" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
         <v>107</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>DE.AE-02</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>108</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>DE.AE-03</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>109</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>DE.AE-04</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
         <v>110</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>DE.AE-06</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
         <v>111</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>DE.AE-07</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
         <v>112</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>DE.AE-08</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="14.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
         <v>113</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="17" t="s">
         <v>114</v>
       </c>
@@ -5644,18 +5644,18 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="29" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="35" t="s">
+    <row r="114" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="B114" s="36"/>
-      <c r="C114" s="29"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="28"/>
       <c r="D114" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
         <v>116</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>RS.MA-01</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
         <v>117</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>RS.MA-02</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
         <v>118</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>RS.MA-03</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
         <v>119</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>RS.MA-04</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>120</v>
       </c>
@@ -5710,18 +5710,18 @@
         <v>RS.MA-05</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="43.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="37" t="s">
+    <row r="120" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="B120" s="36"/>
-      <c r="C120" s="29"/>
+      <c r="B120" s="35"/>
+      <c r="C120" s="28"/>
       <c r="D120" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>122</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>RS.AN-03</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
         <v>123</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>RS.AN-06</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
         <v>124</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>RS.AN-07</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>125</v>
       </c>
@@ -5765,18 +5765,18 @@
         <v>RS.AN-08</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="72" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="35" t="s">
+    <row r="125" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="B125" s="36"/>
-      <c r="C125" s="29"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="28"/>
       <c r="D125" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
         <v>127</v>
       </c>
@@ -5787,7 +5787,7 @@
         <v>RS.CO-02</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
         <v>128</v>
       </c>
@@ -5798,18 +5798,18 @@
         <v>RS.CO-03</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="43.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="37" t="s">
+    <row r="128" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="B128" s="36"/>
-      <c r="C128" s="29"/>
+      <c r="B128" s="35"/>
+      <c r="C128" s="28"/>
       <c r="D128" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="14.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:4" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
         <v>130</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>RS.MI-01</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="14.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:4" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
         <v>131</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>RS.MI-02</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="14.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="s">
         <v>132</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="20" t="s">
         <v>133</v>
       </c>
@@ -5853,18 +5853,18 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="35" t="s">
+    <row r="133" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="B133" s="36"/>
-      <c r="C133" s="29"/>
+      <c r="B133" s="35"/>
+      <c r="C133" s="28"/>
       <c r="D133" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
         <v>135</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>RC.RP-01</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="29" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
         <v>136</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>RC.RP-02</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
         <v>137</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>RC.RP-03</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>138</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>RC.RP-04</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>139</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>RC.RP-05</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>140</v>
       </c>
@@ -5930,18 +5930,18 @@
         <v>RC.RP-06</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="43.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="35" t="s">
+    <row r="140" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="B140" s="36"/>
-      <c r="C140" s="29"/>
+      <c r="B140" s="35"/>
+      <c r="C140" s="28"/>
       <c r="D140" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="57.7" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>142</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>RC.CO-03</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="43.35" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>143</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>RC.CO-04</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="20" t="s">
         <v>144</v>
       </c>
@@ -5997,77 +5997,77 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.35" outlineLevelRow="2" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" style="3" customWidth="1"/>
     <col min="2" max="2" width="36" style="3" customWidth="1"/>
     <col min="3" max="3" width="42" style="3" customWidth="1"/>
     <col min="4" max="4" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.703125" style="3"/>
+    <col min="5" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="33"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39"/>
-    </row>
-    <row r="3" spans="1:4" s="28" customFormat="1" ht="16.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="27" t="s">
+      <c r="C2" s="87"/>
+    </row>
+    <row r="3" spans="1:4" s="27" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="81" t="s">
+    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="102" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="69" t="s">
+    <row r="5" spans="1:4" ht="102" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="180" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:4" ht="182.25" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="89" t="s">
         <v>148</v>
       </c>
       <c r="D6" s="3" t="str">
@@ -6075,1404 +6075,1404 @@
         <v>GV.OC-01</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="53" t="s">
+    <row r="7" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="54"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OC-02</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="51" t="s">
+    <row r="8" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="24"/>
-      <c r="C8" s="55"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OC-03</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="51" t="s">
+    <row r="9" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="24"/>
-      <c r="C9" s="55"/>
+      <c r="C9" s="51"/>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OC-04</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="51" t="s">
+    <row r="10" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="24"/>
-      <c r="C10" s="55"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OC-05</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="87.5" customHeight="1" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="56" t="s">
+    <row r="11" spans="1:4" ht="87.6" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="51" t="s">
+    <row r="12" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="24"/>
-      <c r="C12" s="55"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RM-01</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="51" t="s">
+    <row r="13" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="24"/>
-      <c r="C13" s="55"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RM-02</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="51" t="s">
+    <row r="14" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="24"/>
-      <c r="C14" s="55"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RM-03</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="51" t="s">
+    <row r="15" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="48" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="24"/>
-      <c r="C15" s="55"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RM-04</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="51" t="s">
+    <row r="16" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="24"/>
-      <c r="C16" s="55"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RM-05</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="51" t="s">
+    <row r="17" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="24"/>
-      <c r="C17" s="55"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RM-06</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43" hidden="1" outlineLevel="2" x14ac:dyDescent="0.5">
-      <c r="A18" s="58" t="s">
+    <row r="18" spans="1:4" ht="60" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A18" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="59"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RM-07</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="72" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="60" t="s">
+    <row r="19" spans="1:4" ht="90" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="61"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="53" t="s">
+    <row r="20" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="54"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RR-01</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="51" t="s">
+    <row r="21" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="24"/>
-      <c r="C21" s="55"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RR-02</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="51" t="s">
+    <row r="22" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="48" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="24"/>
-      <c r="C22" s="55"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RR-03</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="58" t="s">
+    <row r="23" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="59"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="55"/>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.RR-04</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.35" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="46" t="s">
+    <row r="24" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="53" t="s">
+    <row r="25" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="54"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.PO-01</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="57.35" hidden="1" outlineLevel="2" x14ac:dyDescent="0.5">
-      <c r="A26" s="58" t="s">
+    <row r="26" spans="1:4" ht="75" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="59"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="55"/>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.PO-02</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="57.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="60" t="s">
+    <row r="27" spans="1:4" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="61"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="53" t="s">
+    <row r="28" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="54"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OV-01</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="51" t="s">
+    <row r="29" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="24"/>
-      <c r="C29" s="55"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OV-02</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="58" t="s">
+    <row r="30" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="59"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.OV-03</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="72" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="46" t="s">
+    <row r="31" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="48"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="53" t="s">
+    <row r="32" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="54"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-01</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="51" t="s">
+    <row r="33" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="48" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="24"/>
-      <c r="C33" s="55"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-02</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="51" t="s">
+    <row r="34" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="24"/>
-      <c r="C34" s="55"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-03</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="51" t="s">
+    <row r="35" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="48" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="24"/>
-      <c r="C35" s="55"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-04</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="72" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="51" t="s">
+    <row r="36" spans="1:4" ht="90.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="24"/>
-      <c r="C36" s="55"/>
+      <c r="C36" s="51"/>
       <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-05</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="51" t="s">
+    <row r="37" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="48" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="24"/>
-      <c r="C37" s="55"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-06</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="72" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="51" t="s">
+    <row r="38" spans="1:4" ht="90.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="48" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="24"/>
-      <c r="C38" s="55"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-07</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="51" t="s">
+    <row r="39" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="24"/>
-      <c r="C39" s="55"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-08</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="72" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="51" t="s">
+    <row r="40" spans="1:4" ht="90.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="48" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="24"/>
-      <c r="C40" s="55"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-09</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="51" t="s">
+    <row r="41" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="48" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="24"/>
-      <c r="C41" s="55"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>GV.SC-10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="62" t="s">
+    <row r="42" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="58" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="5"/>
-      <c r="C42" s="63"/>
+      <c r="C42" s="59"/>
       <c r="D42" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="64" t="s">
+    <row r="43" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="60" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="9"/>
-      <c r="C43" s="65"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="100.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="56" t="s">
+    <row r="44" spans="1:4" ht="120.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="57"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="53"/>
       <c r="D44" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="51" t="s">
+    <row r="45" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="48" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="24"/>
-      <c r="C45" s="55"/>
+      <c r="C45" s="51"/>
       <c r="D45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.AM-01</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="51" t="s">
+    <row r="46" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="48" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="24"/>
-      <c r="C46" s="55"/>
+      <c r="C46" s="51"/>
       <c r="D46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.AM-02</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="51" t="s">
+    <row r="47" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="48" t="s">
         <v>48</v>
       </c>
       <c r="B47" s="24"/>
-      <c r="C47" s="55"/>
+      <c r="C47" s="51"/>
       <c r="D47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.AM-03</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="51" t="s">
+    <row r="48" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="48" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="24"/>
-      <c r="C48" s="55"/>
+      <c r="C48" s="51"/>
       <c r="D48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.AM-04</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="51" t="s">
+    <row r="49" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="48" t="s">
         <v>50</v>
       </c>
       <c r="B49" s="24"/>
-      <c r="C49" s="55"/>
+      <c r="C49" s="51"/>
       <c r="D49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.AM-05</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="51" t="s">
+    <row r="50" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="48" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="24"/>
-      <c r="C50" s="55"/>
+      <c r="C50" s="51"/>
       <c r="D50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.AM-07</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="51" t="s">
+    <row r="51" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="48" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="24"/>
-      <c r="C51" s="55"/>
+      <c r="C51" s="51"/>
       <c r="D51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.AM-08</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="43.35" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="56" t="s">
+    <row r="52" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="66"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="62"/>
       <c r="D52" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="51" t="s">
+    <row r="53" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="48" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="24"/>
-      <c r="C53" s="55"/>
+      <c r="C53" s="51"/>
       <c r="D53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-01</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="51" t="s">
+    <row r="54" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="48" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="24"/>
-      <c r="C54" s="55"/>
+      <c r="C54" s="51"/>
       <c r="D54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-02</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="51" t="s">
+    <row r="55" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="48" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="24"/>
-      <c r="C55" s="55"/>
+      <c r="C55" s="51"/>
       <c r="D55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-03</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="51" t="s">
+    <row r="56" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="48" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="24"/>
-      <c r="C56" s="55"/>
+      <c r="C56" s="51"/>
       <c r="D56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-04</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="51" t="s">
+    <row r="57" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="48" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="24"/>
-      <c r="C57" s="55"/>
+      <c r="C57" s="51"/>
       <c r="D57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-05</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="51" t="s">
+    <row r="58" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="48" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="24"/>
-      <c r="C58" s="55"/>
+      <c r="C58" s="51"/>
       <c r="D58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-06</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="51" t="s">
+    <row r="59" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="48" t="s">
         <v>60</v>
       </c>
       <c r="B59" s="24"/>
-      <c r="C59" s="55"/>
+      <c r="C59" s="51"/>
       <c r="D59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-07</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="51" t="s">
+    <row r="60" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="48" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="24"/>
-      <c r="C60" s="55"/>
+      <c r="C60" s="51"/>
       <c r="D60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-08</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="51" t="s">
+    <row r="61" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="48" t="s">
         <v>62</v>
       </c>
       <c r="B61" s="24"/>
-      <c r="C61" s="55"/>
+      <c r="C61" s="51"/>
       <c r="D61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-09</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="51" t="s">
+    <row r="62" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="48" t="s">
         <v>63</v>
       </c>
       <c r="B62" s="24"/>
-      <c r="C62" s="55"/>
+      <c r="C62" s="51"/>
       <c r="D62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.RA-10</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="57.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="56" t="s">
+    <row r="63" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="34"/>
-      <c r="C63" s="57"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="53"/>
       <c r="D63" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="51" t="s">
+    <row r="64" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="48" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="24"/>
-      <c r="C64" s="55"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.IM-01</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="51" t="s">
+    <row r="65" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="48" t="s">
         <v>66</v>
       </c>
       <c r="B65" s="24"/>
-      <c r="C65" s="55"/>
+      <c r="C65" s="51"/>
       <c r="D65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.IM-02</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="51" t="s">
+    <row r="66" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="48" t="s">
         <v>67</v>
       </c>
       <c r="B66" s="24"/>
-      <c r="C66" s="55"/>
+      <c r="C66" s="51"/>
       <c r="D66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.IM-03</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="51" t="s">
+    <row r="67" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="48" t="s">
         <v>68</v>
       </c>
       <c r="B67" s="24"/>
-      <c r="C67" s="55"/>
+      <c r="C67" s="51"/>
       <c r="D67" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ID.IM-04</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="14.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="67" t="s">
+    <row r="68" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="43"/>
-      <c r="C68" s="68"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="64"/>
       <c r="D68" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="84" t="s">
+    <row r="69" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="85"/>
-      <c r="C69" s="86"/>
+      <c r="B69" s="81"/>
+      <c r="C69" s="82"/>
       <c r="D69" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="86.35" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="69" t="s">
+    <row r="70" spans="1:4" ht="90.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="41"/>
-      <c r="C70" s="70"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="66"/>
       <c r="D70" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="51" t="s">
+    <row r="71" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="48" t="s">
         <v>72</v>
       </c>
       <c r="B71" s="24"/>
-      <c r="C71" s="55"/>
+      <c r="C71" s="51"/>
       <c r="D71" s="3" t="str">
         <f t="shared" ref="D71:D130" si="1">LEFT(A71,8)</f>
         <v>PR.AA-01</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="51" t="s">
+    <row r="72" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="48" t="s">
         <v>73</v>
       </c>
       <c r="B72" s="24"/>
-      <c r="C72" s="55"/>
+      <c r="C72" s="51"/>
       <c r="D72" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.AA-02</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="51" t="s">
+    <row r="73" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="48" t="s">
         <v>74</v>
       </c>
       <c r="B73" s="24"/>
-      <c r="C73" s="55"/>
+      <c r="C73" s="51"/>
       <c r="D73" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.AA-03</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="51" t="s">
+    <row r="74" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="48" t="s">
         <v>75</v>
       </c>
       <c r="B74" s="24"/>
-      <c r="C74" s="55"/>
+      <c r="C74" s="51"/>
       <c r="D74" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.AA-04</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="72" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="51" t="s">
+    <row r="75" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="48" t="s">
         <v>76</v>
       </c>
       <c r="B75" s="24"/>
-      <c r="C75" s="55"/>
+      <c r="C75" s="51"/>
       <c r="D75" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.AA-05</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="51" t="s">
+    <row r="76" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="48" t="s">
         <v>77</v>
       </c>
       <c r="B76" s="24"/>
-      <c r="C76" s="55"/>
+      <c r="C76" s="51"/>
       <c r="D76" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.AA-06</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="72" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="71" t="s">
+    <row r="77" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="36"/>
-      <c r="C77" s="57"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="53"/>
       <c r="D77" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="51" t="s">
+    <row r="78" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="48" t="s">
         <v>79</v>
       </c>
       <c r="B78" s="24"/>
-      <c r="C78" s="55"/>
+      <c r="C78" s="51"/>
       <c r="D78" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.AT-01</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="51" t="s">
+    <row r="79" spans="1:4" ht="75.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="48" t="s">
         <v>80</v>
       </c>
       <c r="B79" s="24"/>
-      <c r="C79" s="55"/>
+      <c r="C79" s="51"/>
       <c r="D79" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.AT-02</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="57.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="56" t="s">
+    <row r="80" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="36"/>
-      <c r="C80" s="66"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="62"/>
       <c r="D80" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="51" t="s">
+    <row r="81" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="48" t="s">
         <v>82</v>
       </c>
       <c r="B81" s="24"/>
-      <c r="C81" s="55"/>
+      <c r="C81" s="51"/>
       <c r="D81" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.DS-01</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="51" t="s">
+    <row r="82" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="48" t="s">
         <v>83</v>
       </c>
       <c r="B82" s="24"/>
-      <c r="C82" s="55"/>
+      <c r="C82" s="51"/>
       <c r="D82" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.DS-02</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="51" t="s">
+    <row r="83" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="48" t="s">
         <v>84</v>
       </c>
       <c r="B83" s="24"/>
-      <c r="C83" s="55"/>
+      <c r="C83" s="51"/>
       <c r="D83" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.DS-10</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="51" t="s">
+    <row r="84" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="48" t="s">
         <v>85</v>
       </c>
       <c r="B84" s="24"/>
-      <c r="C84" s="55"/>
+      <c r="C84" s="51"/>
       <c r="D84" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.DS-11</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="86.35" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="56" t="s">
+    <row r="85" spans="1:4" ht="105.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="36"/>
-      <c r="C85" s="66"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="62"/>
       <c r="D85" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="51" t="s">
+    <row r="86" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="48" t="s">
         <v>87</v>
       </c>
       <c r="B86" s="24"/>
-      <c r="C86" s="55"/>
+      <c r="C86" s="51"/>
       <c r="D86" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.PS-01</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="51" t="s">
+    <row r="87" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="48" t="s">
         <v>88</v>
       </c>
       <c r="B87" s="24"/>
-      <c r="C87" s="55"/>
+      <c r="C87" s="51"/>
       <c r="D87" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.PS-02</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="51" t="s">
+    <row r="88" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="48" t="s">
         <v>89</v>
       </c>
       <c r="B88" s="24"/>
-      <c r="C88" s="55"/>
+      <c r="C88" s="51"/>
       <c r="D88" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.PS-03</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="51" t="s">
+    <row r="89" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="48" t="s">
         <v>90</v>
       </c>
       <c r="B89" s="24"/>
-      <c r="C89" s="55"/>
+      <c r="C89" s="51"/>
       <c r="D89" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.PS-04</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="51" t="s">
+    <row r="90" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="48" t="s">
         <v>91</v>
       </c>
       <c r="B90" s="24"/>
-      <c r="C90" s="55"/>
+      <c r="C90" s="51"/>
       <c r="D90" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.PS-05</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="51" t="s">
+    <row r="91" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="48" t="s">
         <v>92</v>
       </c>
       <c r="B91" s="24"/>
-      <c r="C91" s="55"/>
+      <c r="C91" s="51"/>
       <c r="D91" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.PS-06</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="72" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="56" t="s">
+    <row r="92" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="34"/>
-      <c r="C92" s="57"/>
+      <c r="B92" s="33"/>
+      <c r="C92" s="53"/>
       <c r="D92" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="51" t="s">
+    <row r="93" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B93" s="24"/>
-      <c r="C93" s="55"/>
+      <c r="C93" s="51"/>
       <c r="D93" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.IR-01</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="51" t="s">
+    <row r="94" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="48" t="s">
         <v>95</v>
       </c>
       <c r="B94" s="24"/>
-      <c r="C94" s="55"/>
+      <c r="C94" s="51"/>
       <c r="D94" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.IR-02</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="51" t="s">
+    <row r="95" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="48" t="s">
         <v>96</v>
       </c>
       <c r="B95" s="24"/>
-      <c r="C95" s="55"/>
+      <c r="C95" s="51"/>
       <c r="D95" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.IR-03</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="51" t="s">
+    <row r="96" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="48" t="s">
         <v>97</v>
       </c>
       <c r="B96" s="24"/>
-      <c r="C96" s="55"/>
+      <c r="C96" s="51"/>
       <c r="D96" s="3" t="str">
         <f t="shared" si="1"/>
         <v>PR.IR-04</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="14.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="72" t="s">
+    <row r="97" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="68" t="s">
         <v>98</v>
       </c>
       <c r="B97" s="12"/>
-      <c r="C97" s="73"/>
+      <c r="C97" s="69"/>
       <c r="D97" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="74" t="s">
+    <row r="98" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="70" t="s">
         <v>99</v>
       </c>
       <c r="B98" s="15"/>
-      <c r="C98" s="75"/>
+      <c r="C98" s="71"/>
       <c r="D98" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="56" t="s">
+    <row r="99" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="36"/>
-      <c r="C99" s="66"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="62"/>
       <c r="D99" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="51" t="s">
+    <row r="100" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="48" t="s">
         <v>101</v>
       </c>
       <c r="B100" s="24"/>
-      <c r="C100" s="55"/>
+      <c r="C100" s="51"/>
       <c r="D100" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.CM-01</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="51" t="s">
+    <row r="101" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="48" t="s">
         <v>102</v>
       </c>
       <c r="B101" s="24"/>
-      <c r="C101" s="55"/>
+      <c r="C101" s="51"/>
       <c r="D101" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.CM-02</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="51" t="s">
+    <row r="102" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="48" t="s">
         <v>103</v>
       </c>
       <c r="B102" s="24"/>
-      <c r="C102" s="55"/>
+      <c r="C102" s="51"/>
       <c r="D102" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.CM-03</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="51" t="s">
+    <row r="103" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="48" t="s">
         <v>104</v>
       </c>
       <c r="B103" s="24"/>
-      <c r="C103" s="55"/>
+      <c r="C103" s="51"/>
       <c r="D103" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.CM-06</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="51" t="s">
+    <row r="104" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="48" t="s">
         <v>105</v>
       </c>
       <c r="B104" s="24"/>
-      <c r="C104" s="55"/>
+      <c r="C104" s="51"/>
       <c r="D104" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.CM-09</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="57.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="56" t="s">
+    <row r="105" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="B105" s="34"/>
-      <c r="C105" s="57"/>
+      <c r="B105" s="33"/>
+      <c r="C105" s="53"/>
       <c r="D105" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="51" t="s">
+    <row r="106" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="48" t="s">
         <v>107</v>
       </c>
       <c r="B106" s="24"/>
-      <c r="C106" s="55"/>
+      <c r="C106" s="51"/>
       <c r="D106" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.AE-02</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="51" t="s">
+    <row r="107" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="48" t="s">
         <v>108</v>
       </c>
       <c r="B107" s="24"/>
-      <c r="C107" s="55"/>
+      <c r="C107" s="51"/>
       <c r="D107" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.AE-03</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="51" t="s">
+    <row r="108" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="48" t="s">
         <v>109</v>
       </c>
       <c r="B108" s="24"/>
-      <c r="C108" s="55"/>
+      <c r="C108" s="51"/>
       <c r="D108" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.AE-04</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="51" t="s">
+    <row r="109" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="48" t="s">
         <v>110</v>
       </c>
       <c r="B109" s="24"/>
-      <c r="C109" s="55"/>
+      <c r="C109" s="51"/>
       <c r="D109" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.AE-06</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="51" t="s">
+    <row r="110" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="48" t="s">
         <v>111</v>
       </c>
       <c r="B110" s="24"/>
-      <c r="C110" s="55"/>
+      <c r="C110" s="51"/>
       <c r="D110" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.AE-07</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="51" t="s">
+    <row r="111" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="48" t="s">
         <v>112</v>
       </c>
       <c r="B111" s="24"/>
-      <c r="C111" s="55"/>
+      <c r="C111" s="51"/>
       <c r="D111" s="3" t="str">
         <f t="shared" si="1"/>
         <v>DE.AE-08</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="14.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="74" t="s">
+    <row r="112" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="70" t="s">
         <v>113</v>
       </c>
       <c r="B112" s="15"/>
-      <c r="C112" s="75"/>
+      <c r="C112" s="71"/>
       <c r="D112" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="76" t="s">
+    <row r="113" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="72" t="s">
         <v>114</v>
       </c>
       <c r="B113" s="18"/>
-      <c r="C113" s="77"/>
+      <c r="C113" s="73"/>
       <c r="D113" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="29" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="56" t="s">
+    <row r="114" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="B114" s="36"/>
-      <c r="C114" s="66"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="62"/>
       <c r="D114" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="51" t="s">
+    <row r="115" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="48" t="s">
         <v>116</v>
       </c>
       <c r="B115" s="24"/>
-      <c r="C115" s="55"/>
+      <c r="C115" s="51"/>
       <c r="D115" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.MA-01</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="51" t="s">
+    <row r="116" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="48" t="s">
         <v>117</v>
       </c>
       <c r="B116" s="24"/>
-      <c r="C116" s="55"/>
+      <c r="C116" s="51"/>
       <c r="D116" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.MA-02</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="51" t="s">
+    <row r="117" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="48" t="s">
         <v>118</v>
       </c>
       <c r="B117" s="24"/>
-      <c r="C117" s="55"/>
+      <c r="C117" s="51"/>
       <c r="D117" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.MA-03</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="51" t="s">
+    <row r="118" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="48" t="s">
         <v>119</v>
       </c>
       <c r="B118" s="24"/>
-      <c r="C118" s="55"/>
+      <c r="C118" s="51"/>
       <c r="D118" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.MA-04</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="51" t="s">
+    <row r="119" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="48" t="s">
         <v>120</v>
       </c>
       <c r="B119" s="24"/>
-      <c r="C119" s="55"/>
+      <c r="C119" s="51"/>
       <c r="D119" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.MA-05</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="43.35" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="71" t="s">
+    <row r="120" spans="1:4" ht="60.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="B120" s="36"/>
-      <c r="C120" s="66"/>
+      <c r="B120" s="35"/>
+      <c r="C120" s="62"/>
       <c r="D120" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="51" t="s">
+    <row r="121" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="48" t="s">
         <v>122</v>
       </c>
       <c r="B121" s="24"/>
-      <c r="C121" s="55"/>
+      <c r="C121" s="51"/>
       <c r="D121" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.AN-03</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="51" t="s">
+    <row r="122" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="48" t="s">
         <v>123</v>
       </c>
       <c r="B122" s="24"/>
-      <c r="C122" s="55"/>
+      <c r="C122" s="51"/>
       <c r="D122" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.AN-06</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="51" t="s">
+    <row r="123" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="48" t="s">
         <v>124</v>
       </c>
       <c r="B123" s="24"/>
-      <c r="C123" s="55"/>
+      <c r="C123" s="51"/>
       <c r="D123" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.AN-07</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="51" t="s">
+    <row r="124" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="48" t="s">
         <v>125</v>
       </c>
       <c r="B124" s="24"/>
-      <c r="C124" s="55"/>
+      <c r="C124" s="51"/>
       <c r="D124" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.AN-08</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="72" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="56" t="s">
+    <row r="125" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="B125" s="36"/>
-      <c r="C125" s="66"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="62"/>
       <c r="D125" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="51" t="s">
+    <row r="126" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="48" t="s">
         <v>127</v>
       </c>
       <c r="B126" s="24"/>
-      <c r="C126" s="55"/>
+      <c r="C126" s="51"/>
       <c r="D126" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.CO-02</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="51" t="s">
+    <row r="127" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="48" t="s">
         <v>128</v>
       </c>
       <c r="B127" s="24"/>
-      <c r="C127" s="55"/>
+      <c r="C127" s="51"/>
       <c r="D127" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.CO-03</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="43.35" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="71" t="s">
+    <row r="128" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="B128" s="36"/>
-      <c r="C128" s="66"/>
+      <c r="B128" s="35"/>
+      <c r="C128" s="62"/>
       <c r="D128" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="14.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="51" t="s">
+    <row r="129" spans="1:4" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="48" t="s">
         <v>130</v>
       </c>
       <c r="B129" s="24"/>
-      <c r="C129" s="55"/>
+      <c r="C129" s="51"/>
       <c r="D129" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.MI-01</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="14.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="51" t="s">
+    <row r="130" spans="1:4" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="48" t="s">
         <v>131</v>
       </c>
       <c r="B130" s="24"/>
-      <c r="C130" s="55"/>
+      <c r="C130" s="51"/>
       <c r="D130" s="3" t="str">
         <f t="shared" si="1"/>
         <v>RS.MI-02</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="14.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="76" t="s">
+    <row r="131" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="72" t="s">
         <v>132</v>
       </c>
       <c r="B131" s="18"/>
-      <c r="C131" s="77"/>
+      <c r="C131" s="73"/>
       <c r="D131" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="78" t="s">
+    <row r="132" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="B132" s="79"/>
-      <c r="C132" s="80"/>
+      <c r="B132" s="75"/>
+      <c r="C132" s="76"/>
       <c r="D132" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="57.7" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="40" t="s">
+    <row r="133" spans="1:4" ht="75.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B133" s="49"/>
-      <c r="C133" s="50"/>
+      <c r="B133" s="46"/>
+      <c r="C133" s="47"/>
       <c r="D133" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
         <v>135</v>
       </c>
@@ -7483,7 +7483,7 @@
         <v>RC.RP-01</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="29" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:4" ht="30.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
         <v>136</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>RC.RP-02</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
         <v>137</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>RC.RP-03</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>138</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>RC.RP-04</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>139</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>RC.RP-05</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>140</v>
       </c>
@@ -7538,18 +7538,18 @@
         <v>RC.RP-06</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="43.35" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="35" t="s">
+    <row r="140" spans="1:4" ht="45.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="B140" s="36"/>
-      <c r="C140" s="29"/>
+      <c r="B140" s="35"/>
+      <c r="C140" s="28"/>
       <c r="D140" s="3" t="e">
         <f>LEFT(#REF!,8)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="57.7" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:4" ht="60.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>142</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>RC.CO-03</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="43.35" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:4" ht="45.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>143</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>RC.CO-04</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.7" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:4" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="20" t="s">
         <v>144</v>
       </c>
@@ -7601,6 +7601,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fb85b12d-9ea0-4af7-b89e-54842e89140c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9e79c3b1-452c-4fb6-ac46-d68c59ca6476" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004082676A57B6E94690E98757219CADCB" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f55959268d8877dccd7d02fd6d1da6e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fb85b12d-9ea0-4af7-b89e-54842e89140c" xmlns:ns3="9e79c3b1-452c-4fb6-ac46-d68c59ca6476" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c7ac3f3c4afd4630605d7aa14f2de46" ns2:_="" ns3:_="">
     <xsd:import namespace="fb85b12d-9ea0-4af7-b89e-54842e89140c"/>
@@ -7855,27 +7875,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E921424-0267-41EB-88C0-682153D9F0C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e79c3b1-452c-4fb6-ac46-d68c59ca6476"/>
+    <ds:schemaRef ds:uri="fb85b12d-9ea0-4af7-b89e-54842e89140c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fb85b12d-9ea0-4af7-b89e-54842e89140c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9e79c3b1-452c-4fb6-ac46-d68c59ca6476" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C68428F-BCE9-4CA2-930E-6C21266C294E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E622CBD9-EA8C-46E3-9137-B98E267303DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7892,29 +7917,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C68428F-BCE9-4CA2-930E-6C21266C294E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E921424-0267-41EB-88C0-682153D9F0C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e79c3b1-452c-4fb6-ac46-d68c59ca6476"/>
-    <ds:schemaRef ds:uri="fb85b12d-9ea0-4af7-b89e-54842e89140c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>